<commit_message>
organização restrição geometria fundação
</commit_message>
<xml_diff>
--- a/teste_wand.xlsx
+++ b/teste_wand.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wander\Documents\GitHub\fundaIA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B2790C-780F-465C-9D7C-5842ACA547E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -193,8 +212,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -238,17 +256,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFfff2cc"/>
+        <fgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFe2f0d9"/>
+        <fgColor rgb="FFE2F0D9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffffff"/>
+        <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -262,16 +280,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -286,86 +304,73 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -376,10 +381,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -417,71 +422,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -509,7 +514,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -532,11 +537,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -545,13 +550,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -561,7 +566,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -570,7 +575,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -579,7 +584,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -587,10 +592,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -655,35 +660,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="21" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -733,7 +737,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
@@ -753,7 +757,7 @@
         <v>2.9</v>
       </c>
       <c r="G2" s="12">
-        <v>25.255</v>
+        <v>25.254999999999999</v>
       </c>
       <c r="H2" s="13">
         <v>485.9</v>
@@ -762,7 +766,7 @@
         <v>-0.3</v>
       </c>
       <c r="J2" s="13">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="K2" s="13">
         <v>511.6</v>
@@ -783,7 +787,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
@@ -800,7 +804,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="12">
-        <v>7.985</v>
+        <v>7.9850000000000003</v>
       </c>
       <c r="G3" s="12">
         <v>25.105</v>
@@ -812,13 +816,13 @@
         <v>-1</v>
       </c>
       <c r="J3" s="13">
-        <v>9.2</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="K3" s="13">
         <v>912.1</v>
       </c>
       <c r="L3" s="13">
-        <v>-65.4</v>
+        <v>-65.400000000000006</v>
       </c>
       <c r="M3" s="13">
         <v>0.1</v>
@@ -833,7 +837,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -853,7 +857,7 @@
         <v>13.875</v>
       </c>
       <c r="G4" s="12">
-        <v>25.515</v>
+        <v>25.515000000000001</v>
       </c>
       <c r="H4" s="13">
         <v>1314</v>
@@ -862,7 +866,7 @@
         <v>-3.9</v>
       </c>
       <c r="J4" s="13">
-        <v>20.4</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="K4" s="13">
         <v>1696.4</v>
@@ -883,7 +887,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
@@ -912,7 +916,7 @@
         <v>-3.7</v>
       </c>
       <c r="J5" s="13">
-        <v>9.2</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="K5" s="13">
         <v>891.9</v>
@@ -933,7 +937,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>21</v>
       </c>
@@ -953,7 +957,7 @@
         <v>24.85</v>
       </c>
       <c r="G6" s="12">
-        <v>25.255</v>
+        <v>25.254999999999999</v>
       </c>
       <c r="H6" s="13">
         <v>478.6</v>
@@ -983,7 +987,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row r="7" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
@@ -1006,7 +1010,7 @@
         <v>24.98</v>
       </c>
       <c r="H7" s="13">
-        <v>259.9</v>
+        <v>259.89999999999998</v>
       </c>
       <c r="I7" s="13">
         <v>0.7</v>
@@ -1033,7 +1037,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="8" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
@@ -1083,7 +1087,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row r="9" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
@@ -1133,7 +1137,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row r="10" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
@@ -1150,7 +1154,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="12">
-        <v>19.765</v>
+        <v>19.765000000000001</v>
       </c>
       <c r="G10" s="12">
         <v>19.59</v>
@@ -1183,7 +1187,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row r="11" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
@@ -1203,7 +1207,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="12">
-        <v>18.065</v>
+        <v>18.065000000000001</v>
       </c>
       <c r="H11" s="10">
         <v>230</v>
@@ -1212,7 +1216,7 @@
         <v>1.4</v>
       </c>
       <c r="J11" s="13">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="K11" s="10">
         <v>234</v>
@@ -1233,7 +1237,7 @@
         <v>-4.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row r="12" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>27</v>
       </c>
@@ -1250,13 +1254,13 @@
         <v>17</v>
       </c>
       <c r="F12" s="12">
-        <v>2.305</v>
+        <v>2.3050000000000002</v>
       </c>
       <c r="G12" s="12">
         <v>18.59</v>
       </c>
       <c r="H12" s="13">
-        <v>563.3</v>
+        <v>563.29999999999995</v>
       </c>
       <c r="I12" s="13">
         <v>0.3</v>
@@ -1283,7 +1287,7 @@
         <v>-5.8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row r="13" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>28</v>
       </c>
@@ -1300,7 +1304,7 @@
         <v>17</v>
       </c>
       <c r="F13" s="12">
-        <v>5.205</v>
+        <v>5.2050000000000001</v>
       </c>
       <c r="G13" s="12">
         <v>17.59</v>
@@ -1315,7 +1319,7 @@
         <v>21.2</v>
       </c>
       <c r="K13" s="13">
-        <v>317.9</v>
+        <v>317.89999999999998</v>
       </c>
       <c r="L13" s="13">
         <v>-0.5</v>
@@ -1333,7 +1337,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row r="14" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>29</v>
       </c>
@@ -1353,7 +1357,7 @@
         <v>13.875</v>
       </c>
       <c r="G14" s="12">
-        <v>18.565</v>
+        <v>18.565000000000001</v>
       </c>
       <c r="H14" s="10">
         <v>1071</v>
@@ -1374,16 +1378,16 @@
         <v>0.1</v>
       </c>
       <c r="N14" s="13">
-        <v>1144.1</v>
+        <v>1144.0999999999999</v>
       </c>
       <c r="O14" s="13">
-        <v>72.1</v>
+        <v>72.099999999999994</v>
       </c>
       <c r="P14" s="13">
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row r="15" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
@@ -1406,7 +1410,7 @@
         <v>17.59</v>
       </c>
       <c r="H15" s="13">
-        <v>652.8</v>
+        <v>652.79999999999995</v>
       </c>
       <c r="I15" s="13">
         <v>-0.2</v>
@@ -1424,7 +1428,7 @@
         <v>2.5</v>
       </c>
       <c r="N15" s="13">
-        <v>652.8</v>
+        <v>652.79999999999995</v>
       </c>
       <c r="O15" s="13">
         <v>-0.2</v>
@@ -1433,7 +1437,7 @@
         <v>114.7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row r="16" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
@@ -1468,7 +1472,7 @@
         <v>752.1</v>
       </c>
       <c r="L16" s="13">
-        <v>-142.8</v>
+        <v>-142.80000000000001</v>
       </c>
       <c r="M16" s="13">
         <v>0.3</v>
@@ -1483,7 +1487,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row r="17" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>32</v>
       </c>
@@ -1503,7 +1507,7 @@
         <v>27.75</v>
       </c>
       <c r="G17" s="12">
-        <v>18.065</v>
+        <v>18.065000000000001</v>
       </c>
       <c r="H17" s="13">
         <v>377.3</v>
@@ -1512,7 +1516,7 @@
         <v>-1.9</v>
       </c>
       <c r="J17" s="13">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="K17" s="13">
         <v>259.2</v>
@@ -1533,7 +1537,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row r="18" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>33</v>
       </c>
@@ -1571,7 +1575,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="13">
-        <v>33.2</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="N18" s="13">
         <v>694.2</v>
@@ -1580,10 +1584,10 @@
         <v>0.1</v>
       </c>
       <c r="P18" s="13">
-        <v>-32.2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+        <v>-32.200000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>34</v>
       </c>
@@ -1606,13 +1610,13 @@
         <v>16.395</v>
       </c>
       <c r="H19" s="13">
-        <v>596.2</v>
+        <v>596.20000000000005</v>
       </c>
       <c r="I19" s="13">
         <v>-0.2</v>
       </c>
       <c r="J19" s="13">
-        <v>33.8</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="K19" s="13">
         <v>480.1</v>
@@ -1624,7 +1628,7 @@
         <v>0.3</v>
       </c>
       <c r="N19" s="13">
-        <v>608.8</v>
+        <v>608.79999999999995</v>
       </c>
       <c r="O19" s="13">
         <v>-0.2</v>
@@ -1633,7 +1637,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row r="20" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>35</v>
       </c>
@@ -1683,7 +1687,7 @@
         <v>198.6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row r="21" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>36</v>
       </c>
@@ -1700,7 +1704,7 @@
         <v>17</v>
       </c>
       <c r="F21" s="12">
-        <v>7.534</v>
+        <v>7.5339999999999998</v>
       </c>
       <c r="G21" s="12">
         <v>11.44</v>
@@ -1715,7 +1719,7 @@
         <v>417.6</v>
       </c>
       <c r="K21" s="13">
-        <v>1225.6</v>
+        <v>1225.5999999999999</v>
       </c>
       <c r="L21" s="13">
         <v>430.3</v>
@@ -1733,7 +1737,7 @@
         <v>-384.6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row r="22" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>37</v>
       </c>
@@ -1765,7 +1769,7 @@
         <v>31.5</v>
       </c>
       <c r="K22" s="13">
-        <v>515.7</v>
+        <v>515.70000000000005</v>
       </c>
       <c r="L22" s="13">
         <v>-0.4</v>
@@ -1783,7 +1787,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row r="23" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>38</v>
       </c>
@@ -1833,7 +1837,7 @@
         <v>198.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row r="24" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>39</v>
       </c>
@@ -1871,10 +1875,10 @@
         <v>-0.3</v>
       </c>
       <c r="M24" s="13">
-        <v>32.2</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="N24" s="13">
-        <v>552.8</v>
+        <v>552.79999999999995</v>
       </c>
       <c r="O24" s="10">
         <v>0</v>
@@ -1883,7 +1887,7 @@
         <v>-30.8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>40</v>
       </c>
@@ -1918,7 +1922,7 @@
         <v>470.2</v>
       </c>
       <c r="L25" s="13">
-        <v>-1.1</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="M25" s="13">
         <v>0.2</v>
@@ -1930,10 +1934,10 @@
         <v>-0.1</v>
       </c>
       <c r="P25" s="13">
-        <v>32.2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+        <v>32.200000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>41</v>
       </c>
@@ -1953,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="12">
-        <v>6.640000000000001</v>
+        <v>6.6400000000000006</v>
       </c>
       <c r="H26" s="13">
         <v>236.6</v>
@@ -1962,7 +1966,7 @@
         <v>-0.7</v>
       </c>
       <c r="J26" s="13">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="K26" s="13">
         <v>337.4</v>
@@ -1983,7 +1987,7 @@
         <v>-4.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>42</v>
       </c>
@@ -2000,10 +2004,10 @@
         <v>17</v>
       </c>
       <c r="F27" s="12">
-        <v>2.305</v>
+        <v>2.3050000000000002</v>
       </c>
       <c r="G27" s="12">
-        <v>6.115</v>
+        <v>6.1150000000000002</v>
       </c>
       <c r="H27" s="13">
         <v>557.6</v>
@@ -2033,7 +2037,7 @@
         <v>-5.8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>43</v>
       </c>
@@ -2050,10 +2054,10 @@
         <v>17</v>
       </c>
       <c r="F28" s="12">
-        <v>5.205</v>
+        <v>5.2050000000000001</v>
       </c>
       <c r="G28" s="12">
-        <v>7.115</v>
+        <v>7.1150000000000002</v>
       </c>
       <c r="H28" s="13">
         <v>350.8</v>
@@ -2083,7 +2087,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>44</v>
       </c>
@@ -2103,13 +2107,13 @@
         <v>13.875</v>
       </c>
       <c r="G29" s="12">
-        <v>6.140000000000001</v>
+        <v>6.1400000000000006</v>
       </c>
       <c r="H29" s="10">
         <v>1086</v>
       </c>
       <c r="I29" s="13">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J29" s="10">
         <v>4</v>
@@ -2133,7 +2137,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>45</v>
       </c>
@@ -2153,7 +2157,7 @@
         <v>19.625</v>
       </c>
       <c r="G30" s="12">
-        <v>7.115</v>
+        <v>7.1150000000000002</v>
       </c>
       <c r="H30" s="10">
         <v>683</v>
@@ -2165,7 +2169,7 @@
         <v>114.8</v>
       </c>
       <c r="K30" s="13">
-        <v>633.3</v>
+        <v>633.29999999999995</v>
       </c>
       <c r="L30" s="13">
         <v>-1.2</v>
@@ -2183,7 +2187,7 @@
         <v>114.8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>46</v>
       </c>
@@ -2203,7 +2207,7 @@
         <v>27.75</v>
       </c>
       <c r="G31" s="12">
-        <v>6.115</v>
+        <v>6.1150000000000002</v>
       </c>
       <c r="H31" s="13">
         <v>809.8</v>
@@ -2227,13 +2231,13 @@
         <v>839</v>
       </c>
       <c r="O31" s="13">
-        <v>10.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="P31" s="13">
         <v>6.8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>47</v>
       </c>
@@ -2253,7 +2257,7 @@
         <v>27.75</v>
       </c>
       <c r="G32" s="12">
-        <v>6.640000000000001</v>
+        <v>6.6400000000000006</v>
       </c>
       <c r="H32" s="13">
         <v>377.3</v>
@@ -2283,7 +2287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>48</v>
       </c>
@@ -2303,7 +2307,7 @@
         <v>8.125</v>
       </c>
       <c r="G33" s="12">
-        <v>5.115</v>
+        <v>5.1150000000000002</v>
       </c>
       <c r="H33" s="13">
         <v>895.4</v>
@@ -2333,7 +2337,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row r="34" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>49</v>
       </c>
@@ -2353,7 +2357,7 @@
         <v>19.625</v>
       </c>
       <c r="G34" s="12">
-        <v>5.115</v>
+        <v>5.1150000000000002</v>
       </c>
       <c r="H34" s="13">
         <v>896.7</v>
@@ -2383,7 +2387,7 @@
         <v>112</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>50</v>
       </c>
@@ -2406,16 +2410,16 @@
         <v>0</v>
       </c>
       <c r="H35" s="13">
-        <v>282.6</v>
+        <v>282.60000000000002</v>
       </c>
       <c r="I35" s="13">
         <v>-0.1</v>
       </c>
       <c r="J35" s="13">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="K35" s="13">
-        <v>257.6</v>
+        <v>257.60000000000002</v>
       </c>
       <c r="L35" s="13">
         <v>-30.7</v>
@@ -2427,13 +2431,13 @@
         <v>383.9</v>
       </c>
       <c r="O35" s="13">
-        <v>32.3</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="P35" s="13">
         <v>-0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>51</v>
       </c>
@@ -2483,7 +2487,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>52</v>
       </c>
@@ -2503,7 +2507,7 @@
         <v>2.9</v>
       </c>
       <c r="G37" s="12">
-        <v>-0.55</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="H37" s="13">
         <v>483.6</v>
@@ -2527,13 +2531,13 @@
         <v>526.1</v>
       </c>
       <c r="O37" s="13">
-        <v>32.3</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="P37" s="13">
         <v>-0.7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>53</v>
       </c>
@@ -2550,7 +2554,7 @@
         <v>17</v>
       </c>
       <c r="F38" s="12">
-        <v>7.985</v>
+        <v>7.9850000000000003</v>
       </c>
       <c r="G38" s="12">
         <v>-0.4</v>
@@ -2583,7 +2587,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>54</v>
       </c>
@@ -2621,7 +2625,7 @@
         <v>-232.1</v>
       </c>
       <c r="M39" s="13">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N39" s="10">
         <v>1719</v>
@@ -2633,7 +2637,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>55</v>
       </c>
@@ -2650,7 +2654,7 @@
         <v>17</v>
       </c>
       <c r="F40" s="12">
-        <v>19.765</v>
+        <v>19.765000000000001</v>
       </c>
       <c r="G40" s="12">
         <v>-0.4</v>
@@ -2668,7 +2672,7 @@
         <v>861.3</v>
       </c>
       <c r="L40" s="13">
-        <v>-75.1</v>
+        <v>-75.099999999999994</v>
       </c>
       <c r="M40" s="13">
         <v>0.4</v>
@@ -2683,7 +2687,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>56</v>
       </c>
@@ -2703,7 +2707,7 @@
         <v>25.445</v>
       </c>
       <c r="G41" s="12">
-        <v>-0.55</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="H41" s="13">
         <v>484.6</v>
@@ -2718,22 +2722,22 @@
         <v>436.6</v>
       </c>
       <c r="L41" s="13">
-        <v>-33.2</v>
+        <v>-33.200000000000003</v>
       </c>
       <c r="M41" s="13">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N41" s="13">
-        <v>523.3</v>
+        <v>523.29999999999995</v>
       </c>
       <c r="O41" s="13">
-        <v>35.3</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="P41" s="13">
         <v>0.7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>57</v>
       </c>
@@ -2762,7 +2766,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="13">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="K42" s="10">
         <v>69</v>
@@ -2783,23 +2787,11 @@
         <v>-7.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="15"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="17"/>
+    <row r="43" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D43" s="10"/>
       <c r="E43" s="11"/>
       <c r="F43" s="13"/>
       <c r="G43" s="13"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="16"/>
-      <c r="J43" s="17"/>
-      <c r="K43" s="16"/>
-      <c r="L43" s="17"/>
-      <c r="M43" s="17"/>
-      <c r="N43" s="17"/>
-      <c r="O43" s="16"/>
-      <c r="P43" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat:  dataframe correction, creation app01 streamlit, inserting the result dataframe into the 'obj_ic_fundacoes' and changing the collection of g
</commit_message>
<xml_diff>
--- a/teste_wand.xlsx
+++ b/teste_wand.xlsx
@@ -1,34 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wander\Documents\GitHub\fundaIA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B2790C-780F-465C-9D7C-5842ACA547E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -212,8 +193,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,12 +222,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -256,17 +232,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CC"/>
+        <fgColor rgb="FFfff2cc"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE2F0D9"/>
+        <fgColor rgb="FFe2f0d9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFffffff"/>
       </patternFill>
     </fill>
   </fills>
@@ -280,16 +256,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -304,73 +280,77 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="21">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -381,10 +361,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -422,71 +402,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -514,7 +494,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -537,11 +517,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -550,13 +530,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -566,7 +546,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -575,7 +555,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -584,7 +564,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -592,10 +572,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -660,34 +640,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:P43"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -737,7 +718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
@@ -757,7 +738,7 @@
         <v>2.9</v>
       </c>
       <c r="G2" s="12">
-        <v>25.254999999999999</v>
+        <v>25.255</v>
       </c>
       <c r="H2" s="13">
         <v>485.9</v>
@@ -766,7 +747,7 @@
         <v>-0.3</v>
       </c>
       <c r="J2" s="13">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="K2" s="13">
         <v>511.6</v>
@@ -787,7 +768,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
@@ -804,7 +785,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="12">
-        <v>7.9850000000000003</v>
+        <v>7.985</v>
       </c>
       <c r="G3" s="12">
         <v>25.105</v>
@@ -816,13 +797,13 @@
         <v>-1</v>
       </c>
       <c r="J3" s="13">
-        <v>9.1999999999999993</v>
+        <v>9.2</v>
       </c>
       <c r="K3" s="13">
         <v>912.1</v>
       </c>
       <c r="L3" s="13">
-        <v>-65.400000000000006</v>
+        <v>-65.4</v>
       </c>
       <c r="M3" s="13">
         <v>0.1</v>
@@ -837,7 +818,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -857,7 +838,7 @@
         <v>13.875</v>
       </c>
       <c r="G4" s="12">
-        <v>25.515000000000001</v>
+        <v>25.515</v>
       </c>
       <c r="H4" s="13">
         <v>1314</v>
@@ -866,7 +847,7 @@
         <v>-3.9</v>
       </c>
       <c r="J4" s="13">
-        <v>20.399999999999999</v>
+        <v>20.4</v>
       </c>
       <c r="K4" s="13">
         <v>1696.4</v>
@@ -887,7 +868,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
@@ -916,7 +897,7 @@
         <v>-3.7</v>
       </c>
       <c r="J5" s="13">
-        <v>9.1999999999999993</v>
+        <v>9.2</v>
       </c>
       <c r="K5" s="13">
         <v>891.9</v>
@@ -937,7 +918,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="7" t="s">
         <v>21</v>
       </c>
@@ -957,7 +938,7 @@
         <v>24.85</v>
       </c>
       <c r="G6" s="12">
-        <v>25.254999999999999</v>
+        <v>25.255</v>
       </c>
       <c r="H6" s="13">
         <v>478.6</v>
@@ -987,7 +968,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
@@ -1010,7 +991,7 @@
         <v>24.98</v>
       </c>
       <c r="H7" s="13">
-        <v>259.89999999999998</v>
+        <v>259.9</v>
       </c>
       <c r="I7" s="13">
         <v>0.7</v>
@@ -1037,7 +1018,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
@@ -1087,7 +1068,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
@@ -1137,7 +1118,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
@@ -1154,7 +1135,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="12">
-        <v>19.765000000000001</v>
+        <v>19.765</v>
       </c>
       <c r="G10" s="12">
         <v>19.59</v>
@@ -1187,7 +1168,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
@@ -1207,7 +1188,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="12">
-        <v>18.065000000000001</v>
+        <v>18.065</v>
       </c>
       <c r="H11" s="10">
         <v>230</v>
@@ -1216,7 +1197,7 @@
         <v>1.4</v>
       </c>
       <c r="J11" s="13">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="K11" s="10">
         <v>234</v>
@@ -1237,7 +1218,7 @@
         <v>-4.2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="7" t="s">
         <v>27</v>
       </c>
@@ -1254,13 +1235,13 @@
         <v>17</v>
       </c>
       <c r="F12" s="12">
-        <v>2.3050000000000002</v>
+        <v>2.305</v>
       </c>
       <c r="G12" s="12">
         <v>18.59</v>
       </c>
       <c r="H12" s="13">
-        <v>563.29999999999995</v>
+        <v>563.3</v>
       </c>
       <c r="I12" s="13">
         <v>0.3</v>
@@ -1287,7 +1268,7 @@
         <v>-5.8</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="7" t="s">
         <v>28</v>
       </c>
@@ -1304,7 +1285,7 @@
         <v>17</v>
       </c>
       <c r="F13" s="12">
-        <v>5.2050000000000001</v>
+        <v>5.205</v>
       </c>
       <c r="G13" s="12">
         <v>17.59</v>
@@ -1319,7 +1300,7 @@
         <v>21.2</v>
       </c>
       <c r="K13" s="13">
-        <v>317.89999999999998</v>
+        <v>317.9</v>
       </c>
       <c r="L13" s="13">
         <v>-0.5</v>
@@ -1337,7 +1318,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="7" t="s">
         <v>29</v>
       </c>
@@ -1357,7 +1338,7 @@
         <v>13.875</v>
       </c>
       <c r="G14" s="12">
-        <v>18.565000000000001</v>
+        <v>18.565</v>
       </c>
       <c r="H14" s="10">
         <v>1071</v>
@@ -1378,16 +1359,16 @@
         <v>0.1</v>
       </c>
       <c r="N14" s="13">
-        <v>1144.0999999999999</v>
+        <v>1144.1</v>
       </c>
       <c r="O14" s="13">
-        <v>72.099999999999994</v>
+        <v>72.1</v>
       </c>
       <c r="P14" s="13">
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
@@ -1410,7 +1391,7 @@
         <v>17.59</v>
       </c>
       <c r="H15" s="13">
-        <v>652.79999999999995</v>
+        <v>652.8</v>
       </c>
       <c r="I15" s="13">
         <v>-0.2</v>
@@ -1428,7 +1409,7 @@
         <v>2.5</v>
       </c>
       <c r="N15" s="13">
-        <v>652.79999999999995</v>
+        <v>652.8</v>
       </c>
       <c r="O15" s="13">
         <v>-0.2</v>
@@ -1437,7 +1418,7 @@
         <v>114.7</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
@@ -1472,7 +1453,7 @@
         <v>752.1</v>
       </c>
       <c r="L16" s="13">
-        <v>-142.80000000000001</v>
+        <v>-142.8</v>
       </c>
       <c r="M16" s="13">
         <v>0.3</v>
@@ -1487,7 +1468,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="7" t="s">
         <v>32</v>
       </c>
@@ -1507,7 +1488,7 @@
         <v>27.75</v>
       </c>
       <c r="G17" s="12">
-        <v>18.065000000000001</v>
+        <v>18.065</v>
       </c>
       <c r="H17" s="13">
         <v>377.3</v>
@@ -1516,7 +1497,7 @@
         <v>-1.9</v>
       </c>
       <c r="J17" s="13">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="K17" s="13">
         <v>259.2</v>
@@ -1537,7 +1518,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="7" t="s">
         <v>33</v>
       </c>
@@ -1575,7 +1556,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="13">
-        <v>33.200000000000003</v>
+        <v>33.2</v>
       </c>
       <c r="N18" s="13">
         <v>694.2</v>
@@ -1584,10 +1565,10 @@
         <v>0.1</v>
       </c>
       <c r="P18" s="13">
-        <v>-32.200000000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>-32.2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="7" t="s">
         <v>34</v>
       </c>
@@ -1610,13 +1591,13 @@
         <v>16.395</v>
       </c>
       <c r="H19" s="13">
-        <v>596.20000000000005</v>
+        <v>596.2</v>
       </c>
       <c r="I19" s="13">
         <v>-0.2</v>
       </c>
       <c r="J19" s="13">
-        <v>33.799999999999997</v>
+        <v>33.8</v>
       </c>
       <c r="K19" s="13">
         <v>480.1</v>
@@ -1628,7 +1609,7 @@
         <v>0.3</v>
       </c>
       <c r="N19" s="13">
-        <v>608.79999999999995</v>
+        <v>608.8</v>
       </c>
       <c r="O19" s="13">
         <v>-0.2</v>
@@ -1637,7 +1618,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="7" t="s">
         <v>35</v>
       </c>
@@ -1687,7 +1668,7 @@
         <v>198.6</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="7" t="s">
         <v>36</v>
       </c>
@@ -1704,7 +1685,7 @@
         <v>17</v>
       </c>
       <c r="F21" s="12">
-        <v>7.5339999999999998</v>
+        <v>7.534</v>
       </c>
       <c r="G21" s="12">
         <v>11.44</v>
@@ -1719,7 +1700,7 @@
         <v>417.6</v>
       </c>
       <c r="K21" s="13">
-        <v>1225.5999999999999</v>
+        <v>1225.6</v>
       </c>
       <c r="L21" s="13">
         <v>430.3</v>
@@ -1737,7 +1718,7 @@
         <v>-384.6</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="7" t="s">
         <v>37</v>
       </c>
@@ -1769,7 +1750,7 @@
         <v>31.5</v>
       </c>
       <c r="K22" s="13">
-        <v>515.70000000000005</v>
+        <v>515.7</v>
       </c>
       <c r="L22" s="13">
         <v>-0.4</v>
@@ -1787,7 +1768,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="7" t="s">
         <v>38</v>
       </c>
@@ -1837,7 +1818,7 @@
         <v>198.4</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="7" t="s">
         <v>39</v>
       </c>
@@ -1875,10 +1856,10 @@
         <v>-0.3</v>
       </c>
       <c r="M24" s="13">
-        <v>32.200000000000003</v>
+        <v>32.2</v>
       </c>
       <c r="N24" s="13">
-        <v>552.79999999999995</v>
+        <v>552.8</v>
       </c>
       <c r="O24" s="10">
         <v>0</v>
@@ -1887,7 +1868,7 @@
         <v>-30.8</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="7" t="s">
         <v>40</v>
       </c>
@@ -1922,7 +1903,7 @@
         <v>470.2</v>
       </c>
       <c r="L25" s="13">
-        <v>-1.1000000000000001</v>
+        <v>-1.1</v>
       </c>
       <c r="M25" s="13">
         <v>0.2</v>
@@ -1934,10 +1915,10 @@
         <v>-0.1</v>
       </c>
       <c r="P25" s="13">
-        <v>32.200000000000003</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32.2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="7" t="s">
         <v>41</v>
       </c>
@@ -1957,7 +1938,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="12">
-        <v>6.6400000000000006</v>
+        <v>6.640000000000001</v>
       </c>
       <c r="H26" s="13">
         <v>236.6</v>
@@ -1966,7 +1947,7 @@
         <v>-0.7</v>
       </c>
       <c r="J26" s="13">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="K26" s="13">
         <v>337.4</v>
@@ -1987,7 +1968,7 @@
         <v>-4.2</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="7" t="s">
         <v>42</v>
       </c>
@@ -2004,10 +1985,10 @@
         <v>17</v>
       </c>
       <c r="F27" s="12">
-        <v>2.3050000000000002</v>
+        <v>2.305</v>
       </c>
       <c r="G27" s="12">
-        <v>6.1150000000000002</v>
+        <v>6.115</v>
       </c>
       <c r="H27" s="13">
         <v>557.6</v>
@@ -2037,7 +2018,7 @@
         <v>-5.8</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="7" t="s">
         <v>43</v>
       </c>
@@ -2054,10 +2035,10 @@
         <v>17</v>
       </c>
       <c r="F28" s="12">
-        <v>5.2050000000000001</v>
+        <v>5.205</v>
       </c>
       <c r="G28" s="12">
-        <v>7.1150000000000002</v>
+        <v>7.115</v>
       </c>
       <c r="H28" s="13">
         <v>350.8</v>
@@ -2087,7 +2068,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="7" t="s">
         <v>44</v>
       </c>
@@ -2107,13 +2088,13 @@
         <v>13.875</v>
       </c>
       <c r="G29" s="12">
-        <v>6.1400000000000006</v>
+        <v>6.140000000000001</v>
       </c>
       <c r="H29" s="10">
         <v>1086</v>
       </c>
       <c r="I29" s="13">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="J29" s="10">
         <v>4</v>
@@ -2137,7 +2118,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="7" t="s">
         <v>45</v>
       </c>
@@ -2157,7 +2138,7 @@
         <v>19.625</v>
       </c>
       <c r="G30" s="12">
-        <v>7.1150000000000002</v>
+        <v>7.115</v>
       </c>
       <c r="H30" s="10">
         <v>683</v>
@@ -2169,7 +2150,7 @@
         <v>114.8</v>
       </c>
       <c r="K30" s="13">
-        <v>633.29999999999995</v>
+        <v>633.3</v>
       </c>
       <c r="L30" s="13">
         <v>-1.2</v>
@@ -2187,7 +2168,7 @@
         <v>114.8</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="7" t="s">
         <v>46</v>
       </c>
@@ -2207,7 +2188,7 @@
         <v>27.75</v>
       </c>
       <c r="G31" s="12">
-        <v>6.1150000000000002</v>
+        <v>6.115</v>
       </c>
       <c r="H31" s="13">
         <v>809.8</v>
@@ -2231,13 +2212,13 @@
         <v>839</v>
       </c>
       <c r="O31" s="13">
-        <v>10.199999999999999</v>
+        <v>10.2</v>
       </c>
       <c r="P31" s="13">
         <v>6.8</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="7" t="s">
         <v>47</v>
       </c>
@@ -2257,7 +2238,7 @@
         <v>27.75</v>
       </c>
       <c r="G32" s="12">
-        <v>6.6400000000000006</v>
+        <v>6.640000000000001</v>
       </c>
       <c r="H32" s="13">
         <v>377.3</v>
@@ -2287,7 +2268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="7" t="s">
         <v>48</v>
       </c>
@@ -2307,7 +2288,7 @@
         <v>8.125</v>
       </c>
       <c r="G33" s="12">
-        <v>5.1150000000000002</v>
+        <v>5.115</v>
       </c>
       <c r="H33" s="13">
         <v>895.4</v>
@@ -2337,7 +2318,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="7" t="s">
         <v>49</v>
       </c>
@@ -2357,7 +2338,7 @@
         <v>19.625</v>
       </c>
       <c r="G34" s="12">
-        <v>5.1150000000000002</v>
+        <v>5.115</v>
       </c>
       <c r="H34" s="13">
         <v>896.7</v>
@@ -2387,7 +2368,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="7" t="s">
         <v>50</v>
       </c>
@@ -2410,16 +2391,16 @@
         <v>0</v>
       </c>
       <c r="H35" s="13">
-        <v>282.60000000000002</v>
+        <v>282.6</v>
       </c>
       <c r="I35" s="13">
         <v>-0.1</v>
       </c>
       <c r="J35" s="13">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="K35" s="13">
-        <v>257.60000000000002</v>
+        <v>257.6</v>
       </c>
       <c r="L35" s="13">
         <v>-30.7</v>
@@ -2431,13 +2412,13 @@
         <v>383.9</v>
       </c>
       <c r="O35" s="13">
-        <v>32.299999999999997</v>
+        <v>32.3</v>
       </c>
       <c r="P35" s="13">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="7" t="s">
         <v>51</v>
       </c>
@@ -2487,7 +2468,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="7" t="s">
         <v>52</v>
       </c>
@@ -2507,7 +2488,7 @@
         <v>2.9</v>
       </c>
       <c r="G37" s="12">
-        <v>-0.55000000000000004</v>
+        <v>-0.55</v>
       </c>
       <c r="H37" s="13">
         <v>483.6</v>
@@ -2531,13 +2512,13 @@
         <v>526.1</v>
       </c>
       <c r="O37" s="13">
-        <v>32.299999999999997</v>
+        <v>32.3</v>
       </c>
       <c r="P37" s="13">
         <v>-0.7</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="7" t="s">
         <v>53</v>
       </c>
@@ -2554,7 +2535,7 @@
         <v>17</v>
       </c>
       <c r="F38" s="12">
-        <v>7.9850000000000003</v>
+        <v>7.985</v>
       </c>
       <c r="G38" s="12">
         <v>-0.4</v>
@@ -2587,7 +2568,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="7" t="s">
         <v>54</v>
       </c>
@@ -2625,7 +2606,7 @@
         <v>-232.1</v>
       </c>
       <c r="M39" s="13">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="N39" s="10">
         <v>1719</v>
@@ -2637,7 +2618,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="7" t="s">
         <v>55</v>
       </c>
@@ -2654,7 +2635,7 @@
         <v>17</v>
       </c>
       <c r="F40" s="12">
-        <v>19.765000000000001</v>
+        <v>19.765</v>
       </c>
       <c r="G40" s="12">
         <v>-0.4</v>
@@ -2672,7 +2653,7 @@
         <v>861.3</v>
       </c>
       <c r="L40" s="13">
-        <v>-75.099999999999994</v>
+        <v>-75.1</v>
       </c>
       <c r="M40" s="13">
         <v>0.4</v>
@@ -2687,7 +2668,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="7" t="s">
         <v>56</v>
       </c>
@@ -2707,7 +2688,7 @@
         <v>25.445</v>
       </c>
       <c r="G41" s="12">
-        <v>-0.55000000000000004</v>
+        <v>-0.55</v>
       </c>
       <c r="H41" s="13">
         <v>484.6</v>
@@ -2722,22 +2703,22 @@
         <v>436.6</v>
       </c>
       <c r="L41" s="13">
-        <v>-33.200000000000003</v>
+        <v>-33.2</v>
       </c>
       <c r="M41" s="13">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="N41" s="13">
-        <v>523.29999999999995</v>
+        <v>523.3</v>
       </c>
       <c r="O41" s="13">
-        <v>35.299999999999997</v>
+        <v>35.3</v>
       </c>
       <c r="P41" s="13">
         <v>0.7</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="7" t="s">
         <v>57</v>
       </c>
@@ -2766,7 +2747,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="13">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="K42" s="10">
         <v>69</v>
@@ -2786,12 +2767,6 @@
       <c r="P42" s="13">
         <v>-7.4</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D43" s="10"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: correção verificação geométrica do balanço, pilar_sapata e ppunção
</commit_message>
<xml_diff>
--- a/teste_wand.xlsx
+++ b/teste_wand.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epili\Documents\GitHub\fundaIA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9078A7A-0EBD-4BAC-9CB3-5EA0935B1CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -199,11 +193,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,13 +222,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -247,17 +232,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CC"/>
+        <fgColor rgb="FFfff2cc"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE2F0D9"/>
+        <fgColor rgb="FFe2f0d9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFffffff"/>
       </patternFill>
     </fill>
   </fills>
@@ -271,16 +256,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -292,75 +277,71 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="18">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -371,10 +352,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -412,71 +393,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -504,7 +485,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -527,11 +508,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -540,13 +521,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -556,7 +537,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -565,7 +546,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -574,7 +555,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -582,10 +563,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -650,2130 +631,2131 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="8">
         <v>0.25</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="8">
         <v>1.2</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="9">
         <v>10</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="10">
+      <c r="E2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="11">
         <v>2.9</v>
       </c>
-      <c r="G2" s="10">
-        <v>25.254999999999999</v>
-      </c>
-      <c r="H2" s="11">
+      <c r="G2" s="11">
+        <v>25.255</v>
+      </c>
+      <c r="H2" s="12">
         <v>485.9</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="12">
         <v>-0.3</v>
       </c>
-      <c r="J2" s="11">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="K2" s="11">
+      <c r="J2" s="12">
+        <v>4.1</v>
+      </c>
+      <c r="K2" s="12">
         <v>511.6</v>
       </c>
-      <c r="L2" s="11">
+      <c r="L2" s="12">
         <v>-32.4</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="12">
         <v>-0.4</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="12">
         <v>511.6</v>
       </c>
-      <c r="O2" s="11">
+      <c r="O2" s="12">
         <v>-32.4</v>
       </c>
-      <c r="P2" s="11">
+      <c r="P2" s="12">
         <v>-0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="8">
         <v>0.3</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="8">
         <v>1.5</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="9">
         <v>12</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="10">
-        <v>7.9850000000000003</v>
-      </c>
-      <c r="G3" s="10">
+      <c r="E3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="11">
+        <v>7.985</v>
+      </c>
+      <c r="G3" s="11">
         <v>25.105</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="12">
         <v>885.8</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="9">
         <v>-1</v>
       </c>
-      <c r="J3" s="11">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="K3" s="11">
+      <c r="J3" s="12">
+        <v>9.2</v>
+      </c>
+      <c r="K3" s="12">
         <v>912.1</v>
       </c>
-      <c r="L3" s="11">
-        <v>-65.400000000000006</v>
-      </c>
-      <c r="M3" s="11">
+      <c r="L3" s="12">
+        <v>-65.4</v>
+      </c>
+      <c r="M3" s="12">
         <v>0.1</v>
       </c>
-      <c r="N3" s="11">
+      <c r="N3" s="12">
         <v>915.9</v>
       </c>
-      <c r="O3" s="8">
+      <c r="O3" s="9">
         <v>-40</v>
       </c>
-      <c r="P3" s="11">
+      <c r="P3" s="12">
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="8">
         <v>0.35000000000000003</v>
       </c>
-      <c r="C4" s="18">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="D4" s="8">
+      <c r="C4" s="8">
+        <v>2.32</v>
+      </c>
+      <c r="D4" s="9">
         <v>30</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="10">
+      <c r="E4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="11">
         <v>13.875</v>
       </c>
-      <c r="G4" s="10">
-        <v>25.515000000000001</v>
-      </c>
-      <c r="H4" s="11">
+      <c r="G4" s="11">
+        <v>25.515</v>
+      </c>
+      <c r="H4" s="12">
         <v>1314</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="12">
         <v>-3.9</v>
       </c>
-      <c r="J4" s="11">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="K4" s="11">
+      <c r="J4" s="12">
+        <v>20.4</v>
+      </c>
+      <c r="K4" s="12">
         <v>1696.4</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="12">
         <v>-214.1</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="12">
         <v>0.8</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="12">
         <v>1698.9</v>
       </c>
-      <c r="O4" s="11">
+      <c r="O4" s="12">
         <v>-214.6</v>
       </c>
-      <c r="P4" s="11">
+      <c r="P4" s="12">
         <v>0.7</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="8">
         <v>0.3</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="8">
         <v>1.5</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="9">
         <v>35</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="10">
+      <c r="E5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="11">
         <v>24.85</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="11">
         <v>25.105</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="12">
         <v>855.5</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="12">
         <v>-3.7</v>
       </c>
-      <c r="J5" s="11">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="K5" s="11">
+      <c r="J5" s="12">
+        <v>9.2</v>
+      </c>
+      <c r="K5" s="12">
         <v>891.9</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="9">
         <v>-60</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="12">
         <v>0.6</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="12">
         <v>908.5</v>
       </c>
-      <c r="O5" s="11">
+      <c r="O5" s="12">
         <v>-36.9</v>
       </c>
-      <c r="P5" s="11">
+      <c r="P5" s="12">
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="8">
         <v>0.25</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="8">
         <v>1.2</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="9">
         <v>45</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="10">
+      <c r="E6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="11">
         <v>24.85</v>
       </c>
-      <c r="G6" s="10">
-        <v>25.254999999999999</v>
-      </c>
-      <c r="H6" s="11">
+      <c r="G6" s="11">
+        <v>25.255</v>
+      </c>
+      <c r="H6" s="12">
         <v>478.6</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="12">
         <v>-3.1</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="9">
         <v>5</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="9">
         <v>496</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="12">
         <v>-27.6</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="12">
         <v>0.7</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="9">
         <v>508</v>
       </c>
-      <c r="O6" s="11">
+      <c r="O6" s="12">
         <v>-27.6</v>
       </c>
-      <c r="P6" s="11">
+      <c r="P6" s="12">
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="8">
         <v>0.25</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="8">
         <v>1.75</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="9">
         <v>45</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="12">
+      <c r="E7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="13">
         <v>0</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="11">
         <v>24.98</v>
       </c>
-      <c r="H7" s="11">
-        <v>259.89999999999998</v>
-      </c>
-      <c r="I7" s="11">
+      <c r="H7" s="12">
+        <v>259.9</v>
+      </c>
+      <c r="I7" s="12">
         <v>0.7</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="12">
         <v>5.9</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="12">
         <v>373.8</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="12">
         <v>-85.5</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="12">
         <v>-0.1</v>
       </c>
-      <c r="N7" s="11">
+      <c r="N7" s="12">
         <v>390.8</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="12">
         <v>-85.1</v>
       </c>
-      <c r="P7" s="11">
+      <c r="P7" s="12">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="8">
         <v>0.25</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="8">
         <v>1.75</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="9">
         <v>50</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="10">
+      <c r="E8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="11">
         <v>27.75</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="11">
         <v>24.98</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="12">
         <v>380.8</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="12">
         <v>-6.1</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="12">
         <v>6.2</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="12">
         <v>402.4</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="9">
         <v>-70</v>
       </c>
-      <c r="M8" s="11">
+      <c r="M8" s="12">
         <v>0.5</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N8" s="12">
         <v>402.4</v>
       </c>
-      <c r="O8" s="8">
+      <c r="O8" s="9">
         <v>-70</v>
       </c>
-      <c r="P8" s="11">
+      <c r="P8" s="12">
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="8">
         <v>2.1</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="8">
         <v>0.25</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="9">
         <v>12</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="10">
+      <c r="E9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="11">
         <v>8.125</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="11">
         <v>19.59</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="12">
         <v>857.4</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="12">
         <v>-0.2</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="12">
         <v>115.6</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="9">
         <v>913</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="12">
         <v>-0.9</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M9" s="12">
         <v>0.1</v>
       </c>
-      <c r="N9" s="11">
+      <c r="N9" s="12">
         <v>950.6</v>
       </c>
-      <c r="O9" s="11">
+      <c r="O9" s="12">
         <v>-0.9</v>
       </c>
-      <c r="P9" s="11">
+      <c r="P9" s="12">
         <v>-0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="8">
         <v>2.1</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="8">
         <v>0.25</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="9">
         <v>32</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="10">
-        <v>19.765000000000001</v>
-      </c>
-      <c r="G10" s="10">
+      <c r="E10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="11">
+        <v>19.765</v>
+      </c>
+      <c r="G10" s="11">
         <v>19.59</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="12">
         <v>863.4</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="12">
         <v>-0.2</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="12">
         <v>113.8</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="12">
         <v>863.4</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="12">
         <v>-0.2</v>
       </c>
-      <c r="M10" s="11">
+      <c r="M10" s="12">
         <v>113.8</v>
       </c>
-      <c r="N10" s="11">
+      <c r="N10" s="12">
         <v>903.4</v>
       </c>
-      <c r="O10" s="11">
+      <c r="O10" s="12">
         <v>-0.2</v>
       </c>
-      <c r="P10" s="11">
+      <c r="P10" s="12">
         <v>112.5</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="8">
         <v>0.25</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="8">
         <v>1.2</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="9">
         <v>90</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="12">
+      <c r="E11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="13">
         <v>0</v>
       </c>
-      <c r="G11" s="10">
-        <v>18.065000000000001</v>
-      </c>
-      <c r="H11" s="8">
+      <c r="G11" s="11">
+        <v>18.065</v>
+      </c>
+      <c r="H11" s="9">
         <v>230</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="12">
         <v>1.4</v>
       </c>
-      <c r="J11" s="11">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="K11" s="8">
+      <c r="J11" s="12">
+        <v>4.4</v>
+      </c>
+      <c r="K11" s="9">
         <v>234</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="12">
         <v>-35.4</v>
       </c>
-      <c r="M11" s="8">
+      <c r="M11" s="9">
         <v>0</v>
       </c>
-      <c r="N11" s="11">
+      <c r="N11" s="12">
         <v>366.3</v>
       </c>
-      <c r="O11" s="11">
+      <c r="O11" s="12">
         <v>-0.8</v>
       </c>
-      <c r="P11" s="11">
+      <c r="P11" s="12">
         <v>-4.2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="8">
         <v>0.25</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="8">
         <v>2.25</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="9">
         <v>10</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="10">
-        <v>2.3050000000000002</v>
-      </c>
-      <c r="G12" s="10">
+      <c r="E12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="11">
+        <v>2.305</v>
+      </c>
+      <c r="G12" s="11">
         <v>18.59</v>
       </c>
-      <c r="H12" s="11">
-        <v>563.29999999999995</v>
-      </c>
-      <c r="I12" s="11">
+      <c r="H12" s="12">
+        <v>563.3</v>
+      </c>
+      <c r="I12" s="12">
         <v>0.3</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="12">
         <v>6.2</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="12">
         <v>709.3</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="12">
         <v>-165.3</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="12">
         <v>0.2</v>
       </c>
-      <c r="N12" s="11">
+      <c r="N12" s="12">
         <v>808.4</v>
       </c>
-      <c r="O12" s="11">
+      <c r="O12" s="12">
         <v>-1.2</v>
       </c>
-      <c r="P12" s="11">
+      <c r="P12" s="12">
         <v>-5.8</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="8">
         <v>1.2</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="8">
         <v>0.25</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="9">
         <v>34</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="10">
-        <v>5.2050000000000001</v>
-      </c>
-      <c r="G13" s="10">
+      <c r="E13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="11">
+        <v>5.205</v>
+      </c>
+      <c r="G13" s="11">
         <v>17.59</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="12">
         <v>329.3</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="12">
         <v>0.1</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="12">
         <v>21.2</v>
       </c>
-      <c r="K13" s="11">
-        <v>317.89999999999998</v>
-      </c>
-      <c r="L13" s="11">
+      <c r="K13" s="12">
+        <v>317.9</v>
+      </c>
+      <c r="L13" s="12">
         <v>-0.5</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="12">
         <v>-0.7</v>
       </c>
-      <c r="N13" s="11">
+      <c r="N13" s="12">
         <v>383.1</v>
       </c>
-      <c r="O13" s="11">
+      <c r="O13" s="12">
         <v>0.6</v>
       </c>
-      <c r="P13" s="11">
+      <c r="P13" s="12">
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="8">
         <v>0.3</v>
       </c>
-      <c r="C14" s="18">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D14" s="8">
+      <c r="C14" s="8">
+        <v>2.2</v>
+      </c>
+      <c r="D14" s="9">
         <v>23</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="10">
+      <c r="E14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="11">
         <v>13.875</v>
       </c>
-      <c r="G14" s="10">
-        <v>18.565000000000001</v>
-      </c>
-      <c r="H14" s="8">
+      <c r="G14" s="11">
+        <v>18.565</v>
+      </c>
+      <c r="H14" s="9">
         <v>1071</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I14" s="12">
         <v>-1.4</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="12">
         <v>4.2</v>
       </c>
-      <c r="K14" s="11">
+      <c r="K14" s="12">
         <v>1102.5</v>
       </c>
-      <c r="L14" s="11">
+      <c r="L14" s="12">
         <v>72.3</v>
       </c>
-      <c r="M14" s="11">
+      <c r="M14" s="12">
         <v>0.1</v>
       </c>
-      <c r="N14" s="11">
-        <v>1144.0999999999999</v>
-      </c>
-      <c r="O14" s="11">
-        <v>72.099999999999994</v>
-      </c>
-      <c r="P14" s="11">
+      <c r="N14" s="12">
+        <v>1144.1</v>
+      </c>
+      <c r="O14" s="12">
+        <v>72.1</v>
+      </c>
+      <c r="P14" s="12">
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="8">
         <v>2.1</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="8">
         <v>0.25</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="9">
         <v>12</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="10">
+      <c r="E15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="11">
         <v>19.625</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="11">
         <v>17.59</v>
       </c>
-      <c r="H15" s="11">
-        <v>652.79999999999995</v>
-      </c>
-      <c r="I15" s="11">
+      <c r="H15" s="12">
+        <v>652.8</v>
+      </c>
+      <c r="I15" s="12">
         <v>-0.2</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="12">
         <v>114.7</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15" s="9">
         <v>553</v>
       </c>
-      <c r="L15" s="11">
+      <c r="L15" s="12">
         <v>0.5</v>
       </c>
-      <c r="M15" s="11">
+      <c r="M15" s="12">
         <v>2.5</v>
       </c>
-      <c r="N15" s="11">
-        <v>652.79999999999995</v>
-      </c>
-      <c r="O15" s="11">
+      <c r="N15" s="12">
+        <v>652.8</v>
+      </c>
+      <c r="O15" s="12">
         <v>-0.2</v>
       </c>
-      <c r="P15" s="11">
+      <c r="P15" s="12">
         <v>114.7</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="8">
         <v>0.25</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="8">
         <v>2.25</v>
       </c>
-      <c r="D16" s="8">
-        <v>17</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="10">
+      <c r="D16" s="9">
+        <v>17</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="11">
         <v>25.445</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="11">
         <v>18.59</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="12">
         <v>813.1</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="12">
         <v>-8.1</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="12">
         <v>6.4</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="12">
         <v>752.1</v>
       </c>
-      <c r="L16" s="11">
-        <v>-142.80000000000001</v>
-      </c>
-      <c r="M16" s="11">
+      <c r="L16" s="12">
+        <v>-142.8</v>
+      </c>
+      <c r="M16" s="12">
         <v>0.3</v>
       </c>
-      <c r="N16" s="11">
+      <c r="N16" s="12">
         <v>844.4</v>
       </c>
-      <c r="O16" s="11">
+      <c r="O16" s="12">
         <v>-7.9</v>
       </c>
-      <c r="P16" s="11">
+      <c r="P16" s="12">
         <v>6.4</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="8">
         <v>0.25</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="8">
         <v>1.2</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="9">
         <v>43</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="10">
+      <c r="E17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="11">
         <v>27.75</v>
       </c>
-      <c r="G17" s="10">
-        <v>18.065000000000001</v>
-      </c>
-      <c r="H17" s="11">
+      <c r="G17" s="11">
+        <v>18.065</v>
+      </c>
+      <c r="H17" s="12">
         <v>377.3</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="12">
         <v>-1.9</v>
       </c>
-      <c r="J17" s="11">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="K17" s="11">
+      <c r="J17" s="12">
+        <v>4.4</v>
+      </c>
+      <c r="K17" s="12">
         <v>259.2</v>
       </c>
-      <c r="L17" s="11">
+      <c r="L17" s="12">
         <v>-27.8</v>
       </c>
-      <c r="M17" s="11">
+      <c r="M17" s="12">
         <v>0.1</v>
       </c>
-      <c r="N17" s="11">
+      <c r="N17" s="12">
         <v>383.8</v>
       </c>
-      <c r="O17" s="11">
+      <c r="O17" s="12">
         <v>27.7</v>
       </c>
-      <c r="P17" s="11">
+      <c r="P17" s="12">
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="8">
         <v>1.2</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="8">
         <v>0.3</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="9">
         <v>67</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="10">
+      <c r="E18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="11">
         <v>9.4</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="11">
         <v>16.395</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="12">
         <v>300.2</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="9">
         <v>0</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J18" s="12">
         <v>33.5</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="12">
         <v>302.5</v>
       </c>
-      <c r="L18" s="8">
+      <c r="L18" s="9">
         <v>0</v>
       </c>
-      <c r="M18" s="11">
-        <v>33.200000000000003</v>
-      </c>
-      <c r="N18" s="11">
+      <c r="M18" s="12">
+        <v>33.2</v>
+      </c>
+      <c r="N18" s="12">
         <v>694.2</v>
       </c>
-      <c r="O18" s="11">
+      <c r="O18" s="12">
         <v>0.1</v>
       </c>
-      <c r="P18" s="11">
-        <v>-32.200000000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P18" s="12">
+        <v>-32.2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B19" s="8">
         <v>1.2</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="8">
         <v>0.3</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="9">
         <v>90</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="10">
+      <c r="E19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="11">
         <v>12.08</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="11">
         <v>16.395</v>
       </c>
-      <c r="H19" s="11">
-        <v>596.20000000000005</v>
-      </c>
-      <c r="I19" s="11">
+      <c r="H19" s="12">
+        <v>596.2</v>
+      </c>
+      <c r="I19" s="12">
         <v>-0.2</v>
       </c>
-      <c r="J19" s="11">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="K19" s="11">
+      <c r="J19" s="12">
+        <v>33.8</v>
+      </c>
+      <c r="K19" s="12">
         <v>480.1</v>
       </c>
-      <c r="L19" s="11">
+      <c r="L19" s="12">
         <v>-1.2</v>
       </c>
-      <c r="M19" s="11">
+      <c r="M19" s="12">
         <v>0.3</v>
       </c>
-      <c r="N19" s="11">
-        <v>608.79999999999995</v>
-      </c>
-      <c r="O19" s="11">
+      <c r="N19" s="12">
+        <v>608.8</v>
+      </c>
+      <c r="O19" s="12">
         <v>-0.2</v>
       </c>
-      <c r="P19" s="11">
+      <c r="P19" s="12">
         <v>33.5</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="8">
         <v>1.2</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="8">
         <v>0.25</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="9">
         <v>15</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="10">
+      <c r="E20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="11">
         <v>15.540000000000001</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="11">
         <v>14.552999999999999</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="12">
         <v>1014.4</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="12">
         <v>-61.3</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="12">
         <v>198.6</v>
       </c>
-      <c r="K20" s="11">
+      <c r="K20" s="12">
         <v>1014.4</v>
       </c>
-      <c r="L20" s="11">
+      <c r="L20" s="12">
         <v>-61.3</v>
       </c>
-      <c r="M20" s="11">
+      <c r="M20" s="12">
         <v>198.6</v>
       </c>
-      <c r="N20" s="11">
+      <c r="N20" s="12">
         <v>1014.4</v>
       </c>
-      <c r="O20" s="11">
+      <c r="O20" s="12">
         <v>-61.3</v>
       </c>
-      <c r="P20" s="11">
+      <c r="P20" s="12">
         <v>198.6</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="8">
         <v>1.2</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="8">
         <v>0.25</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="9">
         <v>13</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="10">
-        <v>7.5339999999999998</v>
-      </c>
-      <c r="G21" s="10">
+      <c r="E21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="11">
+        <v>7.534</v>
+      </c>
+      <c r="G21" s="11">
         <v>11.44</v>
       </c>
-      <c r="H21" s="11">
+      <c r="H21" s="12">
         <v>766.7</v>
       </c>
-      <c r="I21" s="11">
+      <c r="I21" s="12">
         <v>-5.4</v>
       </c>
-      <c r="J21" s="11">
+      <c r="J21" s="12">
         <v>417.6</v>
       </c>
-      <c r="K21" s="11">
-        <v>1225.5999999999999</v>
-      </c>
-      <c r="L21" s="11">
+      <c r="K21" s="12">
+        <v>1225.6</v>
+      </c>
+      <c r="L21" s="12">
         <v>430.3</v>
       </c>
-      <c r="M21" s="8">
+      <c r="M21" s="9">
         <v>16</v>
       </c>
-      <c r="N21" s="11">
+      <c r="N21" s="12">
         <v>1733.7</v>
       </c>
-      <c r="O21" s="11">
+      <c r="O21" s="12">
         <v>-3.1</v>
       </c>
-      <c r="P21" s="11">
+      <c r="P21" s="12">
         <v>-384.6</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="8">
         <v>1.2</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="8">
         <v>0.25</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="9">
         <v>14</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="10">
+      <c r="E22" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="11">
         <v>12.08</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="11">
         <v>12.5</v>
       </c>
-      <c r="H22" s="11">
+      <c r="H22" s="12">
         <v>515.9</v>
       </c>
-      <c r="I22" s="11">
+      <c r="I22" s="12">
         <v>0.1</v>
       </c>
-      <c r="J22" s="11">
+      <c r="J22" s="12">
         <v>31.5</v>
       </c>
-      <c r="K22" s="11">
-        <v>515.70000000000005</v>
-      </c>
-      <c r="L22" s="11">
+      <c r="K22" s="12">
+        <v>515.7</v>
+      </c>
+      <c r="L22" s="12">
         <v>-0.4</v>
       </c>
-      <c r="M22" s="11">
+      <c r="M22" s="12">
         <v>-0.1</v>
       </c>
-      <c r="N22" s="11">
+      <c r="N22" s="12">
         <v>515.9</v>
       </c>
-      <c r="O22" s="11">
+      <c r="O22" s="12">
         <v>0.1</v>
       </c>
-      <c r="P22" s="11">
+      <c r="P22" s="12">
         <v>31.5</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="8">
         <v>1.2</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="8">
         <v>0.3</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="9">
         <v>14</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="10">
+      <c r="E23" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="11">
         <v>15.540000000000001</v>
       </c>
-      <c r="G23" s="10">
+      <c r="G23" s="11">
         <v>10.152000000000001</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H23" s="12">
         <v>1006.9</v>
       </c>
-      <c r="I23" s="11">
+      <c r="I23" s="12">
         <v>60.1</v>
       </c>
-      <c r="J23" s="11">
+      <c r="J23" s="12">
         <v>198.4</v>
       </c>
-      <c r="K23" s="11">
+      <c r="K23" s="12">
         <v>616.6</v>
       </c>
-      <c r="L23" s="11">
+      <c r="L23" s="12">
         <v>-58.8</v>
       </c>
-      <c r="M23" s="11">
+      <c r="M23" s="12">
         <v>-187.7</v>
       </c>
-      <c r="N23" s="11">
+      <c r="N23" s="12">
         <v>1006.9</v>
       </c>
-      <c r="O23" s="11">
+      <c r="O23" s="12">
         <v>60.1</v>
       </c>
-      <c r="P23" s="11">
+      <c r="P23" s="12">
         <v>198.4</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="8">
         <v>1.2</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="8">
         <v>0.3</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="9">
         <v>52</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="10">
+      <c r="E24" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="11">
         <v>9.4</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G24" s="11">
         <v>8.32</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="12">
         <v>200.5</v>
       </c>
-      <c r="I24" s="11">
+      <c r="I24" s="12">
         <v>-0.3</v>
       </c>
-      <c r="J24" s="11">
+      <c r="J24" s="12">
         <v>31.9</v>
       </c>
-      <c r="K24" s="11">
+      <c r="K24" s="12">
         <v>228.3</v>
       </c>
-      <c r="L24" s="11">
+      <c r="L24" s="12">
         <v>-0.3</v>
       </c>
-      <c r="M24" s="11">
-        <v>32.200000000000003</v>
-      </c>
-      <c r="N24" s="11">
-        <v>552.79999999999995</v>
-      </c>
-      <c r="O24" s="8">
+      <c r="M24" s="12">
+        <v>32.2</v>
+      </c>
+      <c r="N24" s="12">
+        <v>552.8</v>
+      </c>
+      <c r="O24" s="9">
         <v>0</v>
       </c>
-      <c r="P24" s="11">
+      <c r="P24" s="12">
         <v>-30.8</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="8">
         <v>1.2</v>
       </c>
-      <c r="C25" s="18">
+      <c r="C25" s="8">
         <v>0.3</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="9">
         <v>34</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="10">
+      <c r="E25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="11">
         <v>12.08</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G25" s="11">
         <v>8.32</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="12">
         <v>498.8</v>
       </c>
-      <c r="I25" s="11">
+      <c r="I25" s="12">
         <v>-0.1</v>
       </c>
-      <c r="J25" s="11">
+      <c r="J25" s="12">
         <v>31.9</v>
       </c>
-      <c r="K25" s="11">
+      <c r="K25" s="12">
         <v>470.2</v>
       </c>
-      <c r="L25" s="11">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="M25" s="11">
+      <c r="L25" s="12">
+        <v>-1.1</v>
+      </c>
+      <c r="M25" s="12">
         <v>0.2</v>
       </c>
-      <c r="N25" s="11">
+      <c r="N25" s="12">
         <v>505.7</v>
       </c>
-      <c r="O25" s="11">
+      <c r="O25" s="12">
         <v>-0.1</v>
       </c>
-      <c r="P25" s="11">
-        <v>32.200000000000003</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P25" s="12">
+        <v>32.2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="8">
         <v>0.25</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="8">
         <v>1.2</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="9">
         <v>45</v>
       </c>
-      <c r="E26" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="12">
+      <c r="E26" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="13">
         <v>0</v>
       </c>
-      <c r="G26" s="10">
-        <v>6.6400000000000006</v>
-      </c>
-      <c r="H26" s="11">
+      <c r="G26" s="11">
+        <v>6.640000000000001</v>
+      </c>
+      <c r="H26" s="12">
         <v>236.6</v>
       </c>
-      <c r="I26" s="11">
+      <c r="I26" s="12">
         <v>-0.7</v>
       </c>
-      <c r="J26" s="11">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="K26" s="11">
+      <c r="J26" s="12">
+        <v>4.4</v>
+      </c>
+      <c r="K26" s="12">
         <v>337.4</v>
       </c>
-      <c r="L26" s="11">
+      <c r="L26" s="12">
         <v>-35.1</v>
       </c>
-      <c r="M26" s="8">
+      <c r="M26" s="9">
         <v>0</v>
       </c>
-      <c r="N26" s="11">
+      <c r="N26" s="12">
         <v>369.8</v>
       </c>
-      <c r="O26" s="8">
+      <c r="O26" s="9">
         <v>1</v>
       </c>
-      <c r="P26" s="11">
+      <c r="P26" s="12">
         <v>-4.2</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B27" s="8">
         <v>0.25</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="8">
         <v>2.25</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="9">
         <v>56</v>
       </c>
-      <c r="E27" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="10">
-        <v>2.3050000000000002</v>
-      </c>
-      <c r="G27" s="10">
-        <v>6.1150000000000002</v>
-      </c>
-      <c r="H27" s="11">
+      <c r="E27" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="11">
+        <v>2.305</v>
+      </c>
+      <c r="G27" s="11">
+        <v>6.115</v>
+      </c>
+      <c r="H27" s="12">
         <v>557.6</v>
       </c>
-      <c r="I27" s="11">
+      <c r="I27" s="12">
         <v>1.2</v>
       </c>
-      <c r="J27" s="11">
+      <c r="J27" s="12">
         <v>6.3</v>
       </c>
-      <c r="K27" s="11">
+      <c r="K27" s="12">
         <v>660.2</v>
       </c>
-      <c r="L27" s="11">
+      <c r="L27" s="12">
         <v>-166.2</v>
       </c>
-      <c r="M27" s="11">
+      <c r="M27" s="12">
         <v>0.2</v>
       </c>
-      <c r="N27" s="11">
+      <c r="N27" s="12">
         <v>808.6</v>
       </c>
-      <c r="O27" s="11">
+      <c r="O27" s="12">
         <v>0.5</v>
       </c>
-      <c r="P27" s="11">
+      <c r="P27" s="12">
         <v>-5.8</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="8">
         <v>1.2</v>
       </c>
-      <c r="C28" s="18">
+      <c r="C28" s="8">
         <v>0.25</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="9">
         <v>76</v>
       </c>
-      <c r="E28" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="10">
-        <v>5.2050000000000001</v>
-      </c>
-      <c r="G28" s="10">
-        <v>7.1150000000000002</v>
-      </c>
-      <c r="H28" s="11">
+      <c r="E28" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="11">
+        <v>5.205</v>
+      </c>
+      <c r="G28" s="11">
+        <v>7.115</v>
+      </c>
+      <c r="H28" s="12">
         <v>350.8</v>
       </c>
-      <c r="I28" s="11">
+      <c r="I28" s="12">
         <v>-0.6</v>
       </c>
-      <c r="J28" s="11">
+      <c r="J28" s="12">
         <v>0.4</v>
       </c>
-      <c r="K28" s="11">
+      <c r="K28" s="12">
         <v>350.8</v>
       </c>
-      <c r="L28" s="11">
+      <c r="L28" s="12">
         <v>-0.6</v>
       </c>
-      <c r="M28" s="11">
+      <c r="M28" s="12">
         <v>0.4</v>
       </c>
-      <c r="N28" s="11">
+      <c r="N28" s="12">
         <v>370.2</v>
       </c>
-      <c r="O28" s="11">
+      <c r="O28" s="12">
         <v>-0.6</v>
       </c>
-      <c r="P28" s="11">
+      <c r="P28" s="12">
         <v>0.4</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="8">
         <v>0.3</v>
       </c>
-      <c r="C29" s="18">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D29" s="8">
+      <c r="C29" s="8">
+        <v>2.2</v>
+      </c>
+      <c r="D29" s="9">
         <v>67</v>
       </c>
-      <c r="E29" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F29" s="10">
+      <c r="E29" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="11">
         <v>13.875</v>
       </c>
-      <c r="G29" s="10">
-        <v>6.1400000000000006</v>
-      </c>
-      <c r="H29" s="8">
+      <c r="G29" s="11">
+        <v>6.140000000000001</v>
+      </c>
+      <c r="H29" s="9">
         <v>1086</v>
       </c>
-      <c r="I29" s="11">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J29" s="8">
+      <c r="I29" s="12">
+        <v>1.1</v>
+      </c>
+      <c r="J29" s="9">
         <v>4</v>
       </c>
-      <c r="K29" s="8">
+      <c r="K29" s="9">
         <v>915</v>
       </c>
-      <c r="L29" s="11">
+      <c r="L29" s="12">
         <v>-2.4</v>
       </c>
-      <c r="M29" s="8">
+      <c r="M29" s="9">
         <v>-4</v>
       </c>
-      <c r="N29" s="11">
+      <c r="N29" s="12">
         <v>1090.3</v>
       </c>
-      <c r="O29" s="11">
+      <c r="O29" s="12">
         <v>-82.3</v>
       </c>
-      <c r="P29" s="11">
+      <c r="P29" s="12">
         <v>0.1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="8">
         <v>2.1</v>
       </c>
-      <c r="C30" s="18">
+      <c r="C30" s="8">
         <v>0.25</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="9">
         <v>87</v>
       </c>
-      <c r="E30" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F30" s="10">
+      <c r="E30" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="11">
         <v>19.625</v>
       </c>
-      <c r="G30" s="10">
-        <v>7.1150000000000002</v>
-      </c>
-      <c r="H30" s="8">
+      <c r="G30" s="11">
+        <v>7.115</v>
+      </c>
+      <c r="H30" s="9">
         <v>683</v>
       </c>
-      <c r="I30" s="11">
+      <c r="I30" s="12">
         <v>0.2</v>
       </c>
-      <c r="J30" s="11">
+      <c r="J30" s="12">
         <v>114.8</v>
       </c>
-      <c r="K30" s="11">
-        <v>633.29999999999995</v>
-      </c>
-      <c r="L30" s="11">
+      <c r="K30" s="12">
+        <v>633.3</v>
+      </c>
+      <c r="L30" s="12">
         <v>-1.2</v>
       </c>
-      <c r="M30" s="11">
+      <c r="M30" s="12">
         <v>0.3</v>
       </c>
-      <c r="N30" s="8">
+      <c r="N30" s="9">
         <v>683</v>
       </c>
-      <c r="O30" s="11">
+      <c r="O30" s="12">
         <v>0.2</v>
       </c>
-      <c r="P30" s="11">
+      <c r="P30" s="12">
         <v>114.8</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="18">
+      <c r="B31" s="8">
         <v>0.25</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="8">
         <v>2.25</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="9">
         <v>67</v>
       </c>
-      <c r="E31" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F31" s="10">
+      <c r="E31" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="11">
         <v>27.75</v>
       </c>
-      <c r="G31" s="10">
-        <v>6.1150000000000002</v>
-      </c>
-      <c r="H31" s="11">
+      <c r="G31" s="11">
+        <v>6.115</v>
+      </c>
+      <c r="H31" s="12">
         <v>809.8</v>
       </c>
-      <c r="I31" s="11">
+      <c r="I31" s="12">
         <v>10.8</v>
       </c>
-      <c r="J31" s="11">
+      <c r="J31" s="12">
         <v>6.7</v>
       </c>
-      <c r="K31" s="11">
+      <c r="K31" s="12">
         <v>777.5</v>
       </c>
-      <c r="L31" s="11">
+      <c r="L31" s="12">
         <v>-184.5</v>
       </c>
-      <c r="M31" s="11">
+      <c r="M31" s="12">
         <v>0.2</v>
       </c>
-      <c r="N31" s="8">
+      <c r="N31" s="9">
         <v>839</v>
       </c>
-      <c r="O31" s="11">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="P31" s="11">
+      <c r="O31" s="12">
+        <v>10.2</v>
+      </c>
+      <c r="P31" s="12">
         <v>6.8</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="18">
+      <c r="B32" s="8">
         <v>0.25</v>
       </c>
-      <c r="C32" s="18">
+      <c r="C32" s="8">
         <v>1.2</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="9">
         <v>56</v>
       </c>
-      <c r="E32" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F32" s="10">
+      <c r="E32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="11">
         <v>27.75</v>
       </c>
-      <c r="G32" s="10">
-        <v>6.6400000000000006</v>
-      </c>
-      <c r="H32" s="11">
+      <c r="G32" s="11">
+        <v>6.640000000000001</v>
+      </c>
+      <c r="H32" s="12">
         <v>377.3</v>
       </c>
-      <c r="I32" s="8">
+      <c r="I32" s="9">
         <v>2</v>
       </c>
-      <c r="J32" s="11">
+      <c r="J32" s="12">
         <v>4.7</v>
       </c>
-      <c r="K32" s="8">
+      <c r="K32" s="9">
         <v>354</v>
       </c>
-      <c r="L32" s="11">
+      <c r="L32" s="12">
         <v>-41.6</v>
       </c>
-      <c r="M32" s="8">
+      <c r="M32" s="9">
         <v>0</v>
       </c>
-      <c r="N32" s="11">
+      <c r="N32" s="12">
         <v>384.4</v>
       </c>
-      <c r="O32" s="11">
+      <c r="O32" s="12">
         <v>-41.5</v>
       </c>
-      <c r="P32" s="8">
+      <c r="P32" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="18">
+      <c r="B33" s="8">
         <v>2.1</v>
       </c>
-      <c r="C33" s="18">
+      <c r="C33" s="8">
         <v>0.25</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="9">
         <v>12</v>
       </c>
-      <c r="E33" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" s="10">
+      <c r="E33" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="11">
         <v>8.125</v>
       </c>
-      <c r="G33" s="10">
-        <v>5.1150000000000002</v>
-      </c>
-      <c r="H33" s="11">
+      <c r="G33" s="11">
+        <v>5.115</v>
+      </c>
+      <c r="H33" s="12">
         <v>895.4</v>
       </c>
-      <c r="I33" s="11">
+      <c r="I33" s="12">
         <v>0.2</v>
       </c>
-      <c r="J33" s="11">
+      <c r="J33" s="12">
         <v>114.9</v>
       </c>
-      <c r="K33" s="11">
+      <c r="K33" s="12">
         <v>869.2</v>
       </c>
-      <c r="L33" s="11">
+      <c r="L33" s="12">
         <v>-0.5</v>
       </c>
-      <c r="M33" s="11">
+      <c r="M33" s="12">
         <v>3.5</v>
       </c>
-      <c r="N33" s="11">
+      <c r="N33" s="12">
         <v>950.8</v>
       </c>
-      <c r="O33" s="8">
+      <c r="O33" s="9">
         <v>1</v>
       </c>
-      <c r="P33" s="11">
+      <c r="P33" s="12">
         <v>-0.8</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="18">
+      <c r="B34" s="8">
         <v>2.1</v>
       </c>
-      <c r="C34" s="18">
+      <c r="C34" s="8">
         <v>0.25</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="9">
         <v>56</v>
       </c>
-      <c r="E34" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" s="10">
+      <c r="E34" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="11">
         <v>19.625</v>
       </c>
-      <c r="G34" s="10">
-        <v>5.1150000000000002</v>
-      </c>
-      <c r="H34" s="11">
+      <c r="G34" s="11">
+        <v>5.115</v>
+      </c>
+      <c r="H34" s="12">
         <v>896.7</v>
       </c>
-      <c r="I34" s="11">
+      <c r="I34" s="12">
         <v>0.5</v>
       </c>
-      <c r="J34" s="8">
+      <c r="J34" s="9">
         <v>112</v>
       </c>
-      <c r="K34" s="11">
+      <c r="K34" s="12">
         <v>754.8</v>
       </c>
-      <c r="L34" s="8">
+      <c r="L34" s="9">
         <v>-1</v>
       </c>
-      <c r="M34" s="8">
+      <c r="M34" s="9">
         <v>2</v>
       </c>
-      <c r="N34" s="11">
+      <c r="N34" s="12">
         <v>896.7</v>
       </c>
-      <c r="O34" s="11">
+      <c r="O34" s="12">
         <v>0.5</v>
       </c>
-      <c r="P34" s="8">
+      <c r="P34" s="9">
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="18">
+      <c r="B35" s="8">
         <v>0.25</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35" s="8">
         <v>1.2</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D35" s="9">
         <v>56</v>
       </c>
-      <c r="E35" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F35" s="12">
+      <c r="E35" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="13">
         <v>0</v>
       </c>
-      <c r="G35" s="12">
+      <c r="G35" s="13">
         <v>0</v>
       </c>
-      <c r="H35" s="11">
-        <v>282.60000000000002</v>
-      </c>
-      <c r="I35" s="11">
+      <c r="H35" s="12">
+        <v>282.6</v>
+      </c>
+      <c r="I35" s="12">
         <v>-0.1</v>
       </c>
-      <c r="J35" s="11">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="K35" s="11">
-        <v>257.60000000000002</v>
-      </c>
-      <c r="L35" s="11">
+      <c r="J35" s="12">
+        <v>4.1</v>
+      </c>
+      <c r="K35" s="12">
+        <v>257.6</v>
+      </c>
+      <c r="L35" s="12">
         <v>-30.7</v>
       </c>
-      <c r="M35" s="11">
+      <c r="M35" s="12">
         <v>0.1</v>
       </c>
-      <c r="N35" s="11">
+      <c r="N35" s="12">
         <v>383.9</v>
       </c>
-      <c r="O35" s="11">
-        <v>32.299999999999997</v>
-      </c>
-      <c r="P35" s="11">
+      <c r="O35" s="12">
+        <v>32.3</v>
+      </c>
+      <c r="P35" s="12">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="18">
+      <c r="B36" s="8">
         <v>0.25</v>
       </c>
-      <c r="C36" s="18">
+      <c r="C36" s="8">
         <v>1.2</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D36" s="9">
         <v>56</v>
       </c>
-      <c r="E36" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F36" s="10">
+      <c r="E36" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="11">
         <v>27.75</v>
       </c>
-      <c r="G36" s="12">
+      <c r="G36" s="13">
         <v>0</v>
       </c>
-      <c r="H36" s="11">
+      <c r="H36" s="12">
         <v>367.5</v>
       </c>
-      <c r="I36" s="11">
+      <c r="I36" s="12">
         <v>3.5</v>
       </c>
-      <c r="J36" s="8">
+      <c r="J36" s="9">
         <v>4</v>
       </c>
-      <c r="K36" s="11">
+      <c r="K36" s="12">
         <v>247.1</v>
       </c>
-      <c r="L36" s="11">
+      <c r="L36" s="12">
         <v>-37.4</v>
       </c>
-      <c r="M36" s="11">
+      <c r="M36" s="12">
         <v>0.4</v>
       </c>
-      <c r="N36" s="11">
+      <c r="N36" s="12">
         <v>388.6</v>
       </c>
-      <c r="O36" s="11">
+      <c r="O36" s="12">
         <v>40.5</v>
       </c>
-      <c r="P36" s="11">
+      <c r="P36" s="12">
         <v>-0.2</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="18">
+      <c r="B37" s="8">
         <v>0.25</v>
       </c>
-      <c r="C37" s="18">
+      <c r="C37" s="8">
         <v>1.2</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D37" s="9">
         <v>34</v>
       </c>
-      <c r="E37" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F37" s="10">
+      <c r="E37" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="11">
         <v>2.9</v>
       </c>
-      <c r="G37" s="10">
-        <v>-0.55000000000000004</v>
-      </c>
-      <c r="H37" s="11">
+      <c r="G37" s="11">
+        <v>-0.55</v>
+      </c>
+      <c r="H37" s="12">
         <v>483.6</v>
       </c>
-      <c r="I37" s="11">
+      <c r="I37" s="12">
         <v>0.2</v>
       </c>
-      <c r="J37" s="11">
+      <c r="J37" s="12">
         <v>3.8</v>
       </c>
-      <c r="K37" s="11">
+      <c r="K37" s="12">
         <v>479.1</v>
       </c>
-      <c r="L37" s="11">
+      <c r="L37" s="12">
         <v>-30.6</v>
       </c>
-      <c r="M37" s="11">
+      <c r="M37" s="12">
         <v>-0.5</v>
       </c>
-      <c r="N37" s="11">
+      <c r="N37" s="12">
         <v>526.1</v>
       </c>
-      <c r="O37" s="11">
-        <v>32.299999999999997</v>
-      </c>
-      <c r="P37" s="11">
+      <c r="O37" s="12">
+        <v>32.3</v>
+      </c>
+      <c r="P37" s="12">
         <v>-0.7</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="18">
+      <c r="B38" s="8">
         <v>0.3</v>
       </c>
-      <c r="C38" s="18">
+      <c r="C38" s="8">
         <v>1.5</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D38" s="9">
         <v>29</v>
       </c>
-      <c r="E38" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F38" s="10">
-        <v>7.9850000000000003</v>
-      </c>
-      <c r="G38" s="10">
+      <c r="E38" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="11">
+        <v>7.985</v>
+      </c>
+      <c r="G38" s="11">
         <v>-0.4</v>
       </c>
-      <c r="H38" s="11">
+      <c r="H38" s="12">
         <v>899.5</v>
       </c>
-      <c r="I38" s="11">
+      <c r="I38" s="12">
         <v>0.2</v>
       </c>
-      <c r="J38" s="11">
+      <c r="J38" s="12">
         <v>9.1</v>
       </c>
-      <c r="K38" s="11">
+      <c r="K38" s="12">
         <v>860.6</v>
       </c>
-      <c r="L38" s="11">
+      <c r="L38" s="12">
         <v>-66.7</v>
       </c>
-      <c r="M38" s="11">
+      <c r="M38" s="12">
         <v>0.5</v>
       </c>
-      <c r="N38" s="11">
+      <c r="N38" s="12">
         <v>928.7</v>
       </c>
-      <c r="O38" s="11">
+      <c r="O38" s="12">
         <v>41.7</v>
       </c>
-      <c r="P38" s="11">
+      <c r="P38" s="12">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="18">
+      <c r="B39" s="8">
         <v>0.35000000000000003</v>
       </c>
-      <c r="C39" s="18">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="D39" s="8">
+      <c r="C39" s="8">
+        <v>2.32</v>
+      </c>
+      <c r="D39" s="9">
         <v>34</v>
       </c>
-      <c r="E39" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F39" s="10">
+      <c r="E39" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="11">
         <v>13.875</v>
       </c>
-      <c r="G39" s="10">
+      <c r="G39" s="11">
         <v>-0.81</v>
       </c>
-      <c r="H39" s="11">
+      <c r="H39" s="12">
         <v>1332.1</v>
       </c>
-      <c r="I39" s="11">
+      <c r="I39" s="12">
         <v>0.5</v>
       </c>
-      <c r="J39" s="11">
+      <c r="J39" s="12">
         <v>20.3</v>
       </c>
-      <c r="K39" s="11">
+      <c r="K39" s="12">
         <v>897.2</v>
       </c>
-      <c r="L39" s="11">
+      <c r="L39" s="12">
         <v>-232.1</v>
       </c>
-      <c r="M39" s="11">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="N39" s="8">
+      <c r="M39" s="12">
+        <v>1.1</v>
+      </c>
+      <c r="N39" s="9">
         <v>1719</v>
       </c>
-      <c r="O39" s="11">
+      <c r="O39" s="12">
         <v>232.1</v>
       </c>
-      <c r="P39" s="11">
+      <c r="P39" s="12">
         <v>-0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="18">
+      <c r="B40" s="8">
         <v>0.3</v>
       </c>
-      <c r="C40" s="18">
+      <c r="C40" s="8">
         <v>1.5</v>
       </c>
-      <c r="D40" s="8">
+      <c r="D40" s="9">
         <v>34</v>
       </c>
-      <c r="E40" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F40" s="10">
-        <v>19.765000000000001</v>
-      </c>
-      <c r="G40" s="10">
+      <c r="E40" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="11">
+        <v>19.765</v>
+      </c>
+      <c r="G40" s="11">
         <v>-0.4</v>
       </c>
-      <c r="H40" s="11">
+      <c r="H40" s="12">
         <v>870.9</v>
       </c>
-      <c r="I40" s="11">
+      <c r="I40" s="12">
         <v>2.9</v>
       </c>
-      <c r="J40" s="11">
+      <c r="J40" s="12">
         <v>8.9</v>
       </c>
-      <c r="K40" s="11">
+      <c r="K40" s="12">
         <v>861.3</v>
       </c>
-      <c r="L40" s="11">
-        <v>-75.099999999999994</v>
-      </c>
-      <c r="M40" s="11">
+      <c r="L40" s="12">
+        <v>-75.1</v>
+      </c>
+      <c r="M40" s="12">
         <v>0.4</v>
       </c>
-      <c r="N40" s="11">
+      <c r="N40" s="12">
         <v>928.2</v>
       </c>
-      <c r="O40" s="11">
+      <c r="O40" s="12">
         <v>76.5</v>
       </c>
-      <c r="P40" s="11">
+      <c r="P40" s="12">
         <v>-0.2</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="18">
+      <c r="B41" s="8">
         <v>0.25</v>
       </c>
-      <c r="C41" s="18">
+      <c r="C41" s="8">
         <v>1.2</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D41" s="9">
         <v>34</v>
       </c>
-      <c r="E41" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F41" s="10">
+      <c r="E41" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F41" s="11">
         <v>25.445</v>
       </c>
-      <c r="G41" s="10">
-        <v>-0.55000000000000004</v>
-      </c>
-      <c r="H41" s="11">
+      <c r="G41" s="11">
+        <v>-0.55</v>
+      </c>
+      <c r="H41" s="12">
         <v>484.6</v>
       </c>
-      <c r="I41" s="11">
+      <c r="I41" s="12">
         <v>2.7</v>
       </c>
-      <c r="J41" s="11">
+      <c r="J41" s="12">
         <v>5.3</v>
       </c>
-      <c r="K41" s="11">
+      <c r="K41" s="12">
         <v>436.6</v>
       </c>
-      <c r="L41" s="11">
-        <v>-33.200000000000003</v>
-      </c>
-      <c r="M41" s="11">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="N41" s="11">
-        <v>523.29999999999995</v>
-      </c>
-      <c r="O41" s="11">
-        <v>35.299999999999997</v>
-      </c>
-      <c r="P41" s="11">
+      <c r="L41" s="12">
+        <v>-33.2</v>
+      </c>
+      <c r="M41" s="12">
+        <v>1.1</v>
+      </c>
+      <c r="N41" s="12">
+        <v>523.3</v>
+      </c>
+      <c r="O41" s="12">
+        <v>35.3</v>
+      </c>
+      <c r="P41" s="12">
         <v>0.7</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="18">
+      <c r="B42" s="8">
         <v>0.5</v>
       </c>
-      <c r="C42" s="18">
-        <v>0.2</v>
-      </c>
-      <c r="D42" s="8">
+      <c r="C42" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="D42" s="9">
         <v>34</v>
       </c>
-      <c r="E42" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F42" s="10">
+      <c r="E42" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" s="11">
         <v>0.125</v>
       </c>
-      <c r="G42" s="10">
+      <c r="G42" s="11">
         <v>12.525</v>
       </c>
-      <c r="H42" s="11">
+      <c r="H42" s="12">
         <v>60.3</v>
       </c>
-      <c r="I42" s="8">
+      <c r="I42" s="9">
         <v>0</v>
       </c>
-      <c r="J42" s="11">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="K42" s="8">
+      <c r="J42" s="12">
+        <v>4.6</v>
+      </c>
+      <c r="K42" s="9">
         <v>69</v>
       </c>
-      <c r="L42" s="11">
+      <c r="L42" s="12">
         <v>-0.7</v>
       </c>
-      <c r="M42" s="11">
+      <c r="M42" s="12">
         <v>-1.6</v>
       </c>
-      <c r="N42" s="11">
+      <c r="N42" s="12">
         <v>79.3</v>
       </c>
-      <c r="O42" s="8">
+      <c r="O42" s="9">
         <v>0</v>
       </c>
-      <c r="P42" s="11">
+      <c r="P42" s="12">
         <v>-7.4</v>
       </c>
     </row>

</xml_diff>